<commit_message>
Made Changes for CMS Live
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -64,10 +64,10 @@
     <t xml:space="preserve">UploadAttendeePath</t>
   </si>
   <si>
-    <t xml:space="preserve">Mozila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cmsuat2.event2mobile.com/</t>
+    <t xml:space="preserve">Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cms.event2mobile.com/</t>
   </si>
   <si>
     <t xml:space="preserve">/Users/goni/Documents/workspace/WebSpiders/Event2Mobile/Browser_Driver/geckodriver</t>
@@ -314,8 +314,8 @@
   </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -426,6 +426,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://cms"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Sponsor and Exhibitors Changes
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">BrowserName</t>
   </si>
@@ -76,6 +76,12 @@
     <t xml:space="preserve">MeetingUpload</t>
   </si>
   <si>
+    <t xml:space="preserve">ExhibitorLogo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SponsorsLogo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chrome</t>
   </si>
   <si>
@@ -128,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve">/Test Data/Meeting_Upload.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Test Data/ExhibitorLogo.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Test Data/SponsorLogo.jpg</t>
   </si>
 </sst>
 </file>
@@ -137,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -177,6 +189,13 @@
       <sz val="11"/>
       <color rgb="FF2A00FF"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monaco"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -236,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +285,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,10 +369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,7 +395,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="38.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="48.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="39.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="37.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="34.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="24.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -430,61 +455,73 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leader Board and Analytics added
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">SponsorsLogo</t>
   </si>
   <si>
-    <t xml:space="preserve">Mozila</t>
+    <t xml:space="preserve">Chrome</t>
   </si>
   <si>
     <t xml:space="preserve">https://cms.event2mobile.com/</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">#e2m321</t>
   </si>
   <si>
-    <t xml:space="preserve">Lacity Talent Games 2018</t>
+    <t xml:space="preserve">Real Me Pre Launch Event</t>
   </si>
   <si>
     <t xml:space="preserve">Talent18</t>
@@ -361,8 +361,8 @@
   </sheetPr>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -381,7 +381,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="42.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="38.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="48.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="39.72"/>

</xml_diff>